<commit_message>
The SpritePNGtoCubePixelHelper program can generate all the sprites for all 3 games. Clarified some things for the INFO-6044 Project #1
</commit_message>
<xml_diff>
--- a/6044_FramPat/Projects-Tests/Project #1/SpritePNGtoCubePixelHelper/SpritePNGtoCubePixelHelper/PLY_Models/Defender/Batch_File_Generator.xlsx
+++ b/6044_FramPat/Projects-Tests/Project #1/SpritePNGtoCubePixelHelper/SpritePNGtoCubePixelHelper/PLY_Models/Defender/Batch_File_Generator.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z_FS\00_GDP\2024-2025\GDP202425\6044_FramPat\Projects-Tests\Project #1\SpritePNGtoCubePixelHelper\SpritePNGtoCubePixelHelper\PLY_Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z_FS\00_GDP\2024-2025\GDP202425\6044_FramPat\Projects-Tests\Project #1\SpritePNGtoCubePixelHelper\SpritePNGtoCubePixelHelper\PLY_Models\Defender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB189744-D112-49F3-9061-13EE74518260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DD6828-8655-459E-B03A-187DC31A515B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -296,18 +296,12 @@
     <t>Sprite_Row_7_Col_0_letter_Z.png</t>
   </si>
   <si>
-    <t>../../x64/Release/SpritePNGtoCubePixelHelper.exe</t>
-  </si>
-  <si>
     <t>Exe (relative) Location:</t>
   </si>
   <si>
     <t>PNG (relative) location:</t>
   </si>
   <si>
-    <t>../textures/Defender/Sprites (isolated)</t>
-  </si>
-  <si>
     <t>Test_Crop_Image.png pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</t>
   </si>
   <si>
@@ -318,6 +312,12 @@
   </si>
   <si>
     <t>pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</t>
+  </si>
+  <si>
+    <t>../../../x64/Release/SpritePNGtoCubePixelHelper.exe</t>
+  </si>
+  <si>
+    <t>../../textures/Defender/Sprites (isolated)</t>
   </si>
 </sst>
 </file>
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B91" sqref="B6:B91"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,34 +652,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -688,7 +688,7 @@
       </c>
       <c r="B6" t="str">
         <f>_xlfn.CONCAT("""",$B$1,"""  ","""",$B$2,"/",A6,""""," ",$B$4)</f>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_0_Mutant_1.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_0_Mutant_1.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -697,7 +697,7 @@
       </c>
       <c r="B7" t="str">
         <f t="shared" ref="B7:B70" si="0">_xlfn.CONCAT("""",$B$1,"""  ","""",$B$2,"/",A7,""""," ",$B$4)</f>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_10.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_10.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_11.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_11.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -715,7 +715,7 @@
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_1_Mutant_2.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_1_Mutant_2.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_2.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_2.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -733,7 +733,7 @@
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_3.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_3.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -742,7 +742,7 @@
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_4.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_4.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -751,7 +751,7 @@
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_5.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_5.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -760,7 +760,7 @@
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_6_Astronaut.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_6_Astronaut.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -769,7 +769,7 @@
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_7.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_7.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -778,7 +778,7 @@
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_8.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_8.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -787,7 +787,7 @@
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_9.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_0_Col_9.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -796,7 +796,7 @@
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_0.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_0.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -805,7 +805,7 @@
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_1.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_1.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -814,7 +814,7 @@
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_10.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_10.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -823,7 +823,7 @@
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_11.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_11.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -832,7 +832,7 @@
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_12.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_12.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -841,7 +841,7 @@
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_13.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_13.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -850,7 +850,7 @@
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_2.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_2.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -859,7 +859,7 @@
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_3.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_3.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -868,7 +868,7 @@
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_4.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_4.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -877,7 +877,7 @@
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_5.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_5.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -886,7 +886,7 @@
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_6.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_6.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -895,7 +895,7 @@
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_7.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_7.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -904,7 +904,7 @@
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_8.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_8.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -913,7 +913,7 @@
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_9.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_1_Col_9.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -922,7 +922,7 @@
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_0.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_0.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -931,7 +931,7 @@
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_1.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_1.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -940,7 +940,7 @@
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_2.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_2.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -949,7 +949,7 @@
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_3.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_3.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -958,7 +958,7 @@
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_4.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_4.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -967,7 +967,7 @@
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_5.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_5.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -976,7 +976,7 @@
       </c>
       <c r="B38" t="str">
         <f>_xlfn.CONCAT("""",$B$1,"""  ","""",$B$2,"/",A38,""""," ",$B$4)</f>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_6.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_6.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -985,7 +985,7 @@
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_7.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_7.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -994,7 +994,7 @@
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_8.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_2_Col_8.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_3_Col_0.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_3_Col_0.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1012,7 +1012,7 @@
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_3_Col_1.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_3_Col_1.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_3_Col_2.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_3_Col_2.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_3_Col_3.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_3_Col_3.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_3_Col_4.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_3_Col_4.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_3_Col_5.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_3_Col_5.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1057,7 +1057,7 @@
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_3_Col_6_(250).png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_3_Col_6_(250).png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1066,7 +1066,7 @@
       </c>
       <c r="B48" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_3_Col_7_(250).png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_3_Col_7_(250).png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="B49" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_0.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_0.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1084,7 +1084,7 @@
       </c>
       <c r="B50" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_1.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_1.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_10_number_5.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_10_number_5.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1102,7 +1102,7 @@
       </c>
       <c r="B52" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_11_number_6.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_11_number_6.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1111,7 +1111,7 @@
       </c>
       <c r="B53" t="str">
         <f>_xlfn.CONCAT("""",$B$1,"""  ","""",$B$2,"/",A53,""""," ",$B$4)</f>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_12_number_7.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_12_number_7.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1120,7 +1120,7 @@
       </c>
       <c r="B54" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_13_number_8.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_13_number_8.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1129,7 +1129,7 @@
       </c>
       <c r="B55" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_2_Bang.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_2_Bang.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1138,7 +1138,7 @@
       </c>
       <c r="B56" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_3_decimal_point.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_3_decimal_point.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1147,7 +1147,7 @@
       </c>
       <c r="B57" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_4_apostrophe.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_4_apostrophe.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1156,7 +1156,7 @@
       </c>
       <c r="B58" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_5_number_0.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_5_number_0.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="B59" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_6_number_1.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_6_number_1.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1174,7 +1174,7 @@
       </c>
       <c r="B60" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_7_number_2.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_7_number_2.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="B61" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_8_number_3.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_8_number_3.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B62" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_9_number_4.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_4_Col_9_number_4.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="B63" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_0_number_9.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_0_number_9.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="B64" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_10_letter_H.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_10_letter_H.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1219,7 +1219,7 @@
       </c>
       <c r="B65" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_10_letter_I.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_10_letter_I.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="B66" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_10_letter_J.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_10_letter_J.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1237,7 +1237,7 @@
       </c>
       <c r="B67" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_10_letter_K.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_10_letter_K.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1246,7 +1246,7 @@
       </c>
       <c r="B68" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_1_colon.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_1_colon.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="B69" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_2_question_mark.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_2_question_mark.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="B70" t="str">
         <f t="shared" si="0"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_3_letter_A.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_3_letter_A.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="B71" t="str">
         <f t="shared" ref="B71:B91" si="1">_xlfn.CONCAT("""",$B$1,"""  ","""",$B$2,"/",A71,""""," ",$B$4)</f>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_4_letter_B.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_4_letter_B.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1282,7 +1282,7 @@
       </c>
       <c r="B72" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_5_letter_C.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_5_letter_C.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="B73" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_6_letter_D.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_6_letter_D.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="B74" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_7_letter_E.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_7_letter_E.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="B75" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_8_letter_F.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_8_letter_F.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="B76" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_9_letter_G.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_5_Col_9_letter_G.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1327,7 +1327,7 @@
       </c>
       <c r="B77" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_0_letter_L.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_0_letter_L.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1336,7 +1336,7 @@
       </c>
       <c r="B78" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_10_letter_V.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_10_letter_V.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1345,7 +1345,7 @@
       </c>
       <c r="B79" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_11_letter_W.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_11_letter_W.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1354,7 +1354,7 @@
       </c>
       <c r="B80" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_12_letter_X.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_12_letter_X.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="B81" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_1_letter_M.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_1_letter_M.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="B82" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_2_letter_N.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_2_letter_N.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B83" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_3_letter_O.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_3_letter_O.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1390,7 +1390,7 @@
       </c>
       <c r="B84" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_4_letter_P.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_4_letter_P.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1399,7 +1399,7 @@
       </c>
       <c r="B85" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_5_letter_Q.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_5_letter_Q.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="B86" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_6_letter_R.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_6_letter_R.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="B87" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_7_letter_S.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_7_letter_S.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1426,7 +1426,7 @@
       </c>
       <c r="B88" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_8_letter_T.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_8_letter_T.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="B89" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_9_letter_U.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_6_Col_9_letter_U.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1444,7 +1444,7 @@
       </c>
       <c r="B90" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_7_Col_0_letter_Y.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_7_Col_0_letter_Y.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="B91" t="str">
         <f t="shared" si="1"/>
-        <v>"../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../textures/Defender/Sprites (isolated)/Sprite_Row_7_Col_0_letter_Z.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
+        <v>"../../../x64/Release/SpritePNGtoCubePixelHelper.exe"  "../../textures/Defender/Sprites (isolated)/Sprite_Row_7_Col_0_letter_Z.png" pixelSize:4 setBackgroundColour:0:0:0 cropToBackgroundColour noBackgroundColourBlocks</v>
       </c>
     </row>
   </sheetData>

</xml_diff>